<commit_message>
Refining alignments and tabular for parvovirus reference set
</commit_message>
<xml_diff>
--- a/tabular/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/parvo-ncbi-refseqs-side-data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="98">
   <si>
     <t>accession-ID</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>MpBuV</t>
-  </si>
-  <si>
-    <t>Bufaparvovirus</t>
   </si>
   <si>
     <t>NC_006259</t>
@@ -411,8 +408,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -426,11 +425,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -763,7 +764,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -784,7 +785,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -793,55 +794,55 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>64</v>
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>64</v>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>86</v>
@@ -850,301 +851,301 @@
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>64</v>
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>64</v>
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>64</v>
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="F11" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>64</v>
+      <c r="C12" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>64</v>
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>64</v>
+      <c r="A14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>64</v>
+      <c r="A15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>27</v>
@@ -1153,150 +1154,155 @@
         <v>44</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>64</v>
+      <c r="A20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="4" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" t="s">
-        <v>95</v>
+      <c r="A26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E26" t="s">
-        <v>97</v>
+      <c r="E26" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F26">
+    <sortCondition ref="D2:D26"/>
+    <sortCondition ref="E2:E26"/>
+    <sortCondition ref="B2:B26"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Updated build to bring in more alignments
</commit_message>
<xml_diff>
--- a/tabular/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/parvo-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="1880" windowWidth="27880" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="22260" yWindow="4280" windowWidth="27880" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal refset" sheetId="2" r:id="rId1"/>
@@ -319,7 +319,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -372,8 +372,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,6 +405,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -408,7 +420,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -416,22 +428,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -761,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1297,6 +1316,9 @@
         <v>63</v>
       </c>
     </row>
+    <row r="30" spans="1:6">
+      <c r="D30" s="6"/>
+    </row>
   </sheetData>
   <sortState ref="A2:F26">
     <sortCondition ref="D2:D26"/>

</xml_diff>

<commit_message>
Updated alignments - near complete parvovirinae alignment tree with seven of eight genera. Also added chappa
</commit_message>
<xml_diff>
--- a/tabular/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/parvo-ncbi-refseqs-side-data.xlsx
@@ -420,7 +420,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -429,6 +429,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -441,16 +451,26 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="20">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="7" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -783,7 +803,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="F26" sqref="A1:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Updated project build (fully validated)
</commit_message>
<xml_diff>
--- a/tabular/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/parvo-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22260" yWindow="4280" windowWidth="27880" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="15620" yWindow="1360" windowWidth="27880" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal refset" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="142">
   <si>
     <t>accession-ID</t>
   </si>
@@ -313,13 +313,145 @@
   </si>
   <si>
     <t>KX907333</t>
+  </si>
+  <si>
+    <t>AF221122</t>
+  </si>
+  <si>
+    <t>AF221123</t>
+  </si>
+  <si>
+    <t>AF321230</t>
+  </si>
+  <si>
+    <t>AF406967</t>
+  </si>
+  <si>
+    <t>AY622943</t>
+  </si>
+  <si>
+    <t>D00623</t>
+  </si>
+  <si>
+    <t>EU200669</t>
+  </si>
+  <si>
+    <t>EU200677</t>
+  </si>
+  <si>
+    <t>EU659112</t>
+  </si>
+  <si>
+    <t>EU659120</t>
+  </si>
+  <si>
+    <t>GQ200736</t>
+  </si>
+  <si>
+    <t>GU938300</t>
+  </si>
+  <si>
+    <t>HQ113143</t>
+  </si>
+  <si>
+    <t>JF429835</t>
+  </si>
+  <si>
+    <t>JF504699</t>
+  </si>
+  <si>
+    <t>JN202450</t>
+  </si>
+  <si>
+    <t>JN420361</t>
+  </si>
+  <si>
+    <t>JX505432</t>
+  </si>
+  <si>
+    <t>JX885610</t>
+  </si>
+  <si>
+    <t>KJ396349</t>
+  </si>
+  <si>
+    <t>KJ396350</t>
+  </si>
+  <si>
+    <t>KJ396352</t>
+  </si>
+  <si>
+    <t>KJ641666</t>
+  </si>
+  <si>
+    <t>KT965075</t>
+  </si>
+  <si>
+    <t>MF682922</t>
+  </si>
+  <si>
+    <t>MF682923</t>
+  </si>
+  <si>
+    <t>MF682925</t>
+  </si>
+  <si>
+    <t>MG745669</t>
+  </si>
+  <si>
+    <t>MG745671</t>
+  </si>
+  <si>
+    <t>MG972981</t>
+  </si>
+  <si>
+    <t>NC_012042</t>
+  </si>
+  <si>
+    <t>NC_015718</t>
+  </si>
+  <si>
+    <t>NC_020499</t>
+  </si>
+  <si>
+    <t>NC_025825</t>
+  </si>
+  <si>
+    <t>NC_025891</t>
+  </si>
+  <si>
+    <t>NC_026251</t>
+  </si>
+  <si>
+    <t>NC_028136</t>
+  </si>
+  <si>
+    <t>NC_029797</t>
+  </si>
+  <si>
+    <t>NC_030837</t>
+  </si>
+  <si>
+    <t>NC_031450</t>
+  </si>
+  <si>
+    <t>NC_031670</t>
+  </si>
+  <si>
+    <t>NC_031695</t>
+  </si>
+  <si>
+    <t>NC_034445</t>
+  </si>
+  <si>
+    <t>U26342</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -372,15 +504,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,11 +530,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -420,7 +540,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -428,7 +548,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -442,35 +563,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="Good" xfId="7" builtinId="26"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -800,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="A1:F26"/>
+      <selection activeCell="F70" sqref="B11:F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1336,8 +1457,357 @@
         <v>63</v>
       </c>
     </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="30" spans="1:6">
-      <c r="D30" s="6"/>
+      <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>111</v>
+      </c>
+      <c r="F40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>112</v>
+      </c>
+      <c r="F41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>116</v>
+      </c>
+      <c r="F45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>118</v>
+      </c>
+      <c r="F47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" t="s">
+        <v>119</v>
+      </c>
+      <c r="F48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>120</v>
+      </c>
+      <c r="F49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
+        <v>121</v>
+      </c>
+      <c r="F50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>122</v>
+      </c>
+      <c r="F51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>123</v>
+      </c>
+      <c r="F52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
+        <v>125</v>
+      </c>
+      <c r="F54" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
+        <v>127</v>
+      </c>
+      <c r="F56" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
+        <v>128</v>
+      </c>
+      <c r="F57" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
+        <v>129</v>
+      </c>
+      <c r="F58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>130</v>
+      </c>
+      <c r="F59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>131</v>
+      </c>
+      <c r="F60" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>132</v>
+      </c>
+      <c r="F61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>133</v>
+      </c>
+      <c r="F62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>134</v>
+      </c>
+      <c r="F63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>135</v>
+      </c>
+      <c r="F64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>136</v>
+      </c>
+      <c r="F65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>137</v>
+      </c>
+      <c r="F66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>138</v>
+      </c>
+      <c r="F67" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
+        <v>139</v>
+      </c>
+      <c r="F68" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>140</v>
+      </c>
+      <c r="F69" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>141</v>
+      </c>
+      <c r="F70" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:F26">

</xml_diff>

<commit_message>
Updated tabular info - added chapparvos
</commit_message>
<xml_diff>
--- a/tabular/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/parvo-ncbi-refseqs-side-data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="149">
   <si>
     <t>accession-ID</t>
   </si>
@@ -445,13 +445,34 @@
   </si>
   <si>
     <t>U26342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cebus_imitator.1               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mesitornis_unicolor.1          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myotis_davidii.1               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protobothrops_mucrosquamatus.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serinus_canaria.1           </t>
+  </si>
+  <si>
+    <t>fasta</t>
+  </si>
+  <si>
+    <t>Chapparvovirinae</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -504,6 +525,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -540,7 +569,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -562,16 +591,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -582,6 +624,12 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -592,6 +640,12 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -921,15 +975,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F70" sqref="B11:F70"/>
+      <selection activeCell="F1" sqref="A1:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="28.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
@@ -937,7 +991,7 @@
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -957,301 +1011,306 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4" t="s">
+      <c r="F12" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E13" t="s">
-        <v>96</v>
+      <c r="E13" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:10">
       <c r="A14" s="4" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:10">
       <c r="A15" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:10">
       <c r="A16" s="4" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>63</v>
@@ -1259,39 +1318,39 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>53</v>
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>44</v>
+      <c r="E18" t="s">
+        <v>96</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>63</v>
@@ -1299,19 +1358,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>63</v>
@@ -1319,19 +1378,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>69</v>
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>63</v>
@@ -1339,19 +1398,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>63</v>
@@ -1359,19 +1418,19 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>63</v>
@@ -1379,19 +1438,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>63</v>
@@ -1399,19 +1458,19 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>58</v>
+        <v>93</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>63</v>
@@ -1419,19 +1478,19 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>63</v>
@@ -1439,67 +1498,127 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>99</v>
-      </c>
-      <c r="F28" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>100</v>
-      </c>
-      <c r="F29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>102</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="F31" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F32" t="s">
         <v>63</v>
@@ -1507,7 +1626,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F33" t="s">
         <v>63</v>
@@ -1515,7 +1634,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F34" t="s">
         <v>63</v>
@@ -1523,7 +1642,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F35" t="s">
         <v>63</v>
@@ -1531,7 +1650,7 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F36" t="s">
         <v>63</v>
@@ -1539,7 +1658,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F37" t="s">
         <v>63</v>
@@ -1547,7 +1666,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="F38" t="s">
         <v>63</v>
@@ -1555,7 +1674,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F39" t="s">
         <v>63</v>
@@ -1563,7 +1682,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F40" t="s">
         <v>63</v>
@@ -1571,7 +1690,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F41" t="s">
         <v>63</v>
@@ -1579,7 +1698,7 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F42" t="s">
         <v>63</v>
@@ -1587,7 +1706,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F43" t="s">
         <v>63</v>
@@ -1595,7 +1714,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F44" t="s">
         <v>63</v>
@@ -1603,7 +1722,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F45" t="s">
         <v>63</v>
@@ -1611,7 +1730,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F46" t="s">
         <v>63</v>
@@ -1619,7 +1738,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F47" t="s">
         <v>63</v>
@@ -1627,7 +1746,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F48" t="s">
         <v>63</v>
@@ -1635,7 +1754,7 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F49" t="s">
         <v>63</v>
@@ -1643,7 +1762,7 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F50" t="s">
         <v>63</v>
@@ -1651,7 +1770,7 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F51" t="s">
         <v>63</v>
@@ -1659,7 +1778,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F52" t="s">
         <v>63</v>
@@ -1667,7 +1786,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F53" t="s">
         <v>63</v>
@@ -1675,7 +1794,7 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F54" t="s">
         <v>63</v>
@@ -1683,7 +1802,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F55" t="s">
         <v>63</v>
@@ -1691,7 +1810,7 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F56" t="s">
         <v>63</v>
@@ -1699,7 +1818,7 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F57" t="s">
         <v>63</v>
@@ -1707,7 +1826,7 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F58" t="s">
         <v>63</v>
@@ -1715,7 +1834,7 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F59" t="s">
         <v>63</v>
@@ -1723,7 +1842,7 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F60" t="s">
         <v>63</v>
@@ -1731,7 +1850,7 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F61" t="s">
         <v>63</v>
@@ -1739,7 +1858,7 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F62" t="s">
         <v>63</v>
@@ -1747,7 +1866,7 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F63" t="s">
         <v>63</v>
@@ -1755,7 +1874,7 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F64" t="s">
         <v>63</v>
@@ -1763,7 +1882,7 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F65" t="s">
         <v>63</v>
@@ -1771,7 +1890,7 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F66" t="s">
         <v>63</v>
@@ -1779,7 +1898,7 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F67" t="s">
         <v>63</v>
@@ -1787,7 +1906,7 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F68" t="s">
         <v>63</v>
@@ -1795,7 +1914,7 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F69" t="s">
         <v>63</v>
@@ -1803,9 +1922,49 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
+        <v>136</v>
+      </c>
+      <c r="F70" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
+        <v>137</v>
+      </c>
+      <c r="F71" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" t="s">
+        <v>138</v>
+      </c>
+      <c r="F72" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>139</v>
+      </c>
+      <c r="F73" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>140</v>
+      </c>
+      <c r="F74" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="14" customHeight="1">
+      <c r="A75" t="s">
         <v>141</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F75" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added fully annotated reference sequence set
</commit_message>
<xml_diff>
--- a/tabular/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/parvo-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="900" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="15860" yWindow="5300" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal refset" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="268">
   <si>
     <t>accession-ID</t>
   </si>
@@ -512,6 +512,318 @@
   </si>
   <si>
     <t>Hipposideros pomona</t>
+  </si>
+  <si>
+    <t>Gray fox amdovirus</t>
+  </si>
+  <si>
+    <t>Urocyon cinereoargenteus</t>
+  </si>
+  <si>
+    <t>JN202450</t>
+  </si>
+  <si>
+    <t>GF-AmdoPV</t>
+  </si>
+  <si>
+    <t>Skunk amdoparvovirus</t>
+  </si>
+  <si>
+    <t>SK-AmdoPV</t>
+  </si>
+  <si>
+    <t>NC_034445</t>
+  </si>
+  <si>
+    <t>Arctic fox amdovirus</t>
+  </si>
+  <si>
+    <t>KJ396352</t>
+  </si>
+  <si>
+    <t>ArcFox-Amdo-PV</t>
+  </si>
+  <si>
+    <t>Vulpes lagopus</t>
+  </si>
+  <si>
+    <t>Enhydra lutris</t>
+  </si>
+  <si>
+    <t>Rousettus leschenaultii bocaparvovirus 1</t>
+  </si>
+  <si>
+    <t>Rousettus leschenaultii</t>
+  </si>
+  <si>
+    <t>Rl-BocaPV-1</t>
+  </si>
+  <si>
+    <t>MF682925</t>
+  </si>
+  <si>
+    <t>California sea lion bocavirus 1</t>
+  </si>
+  <si>
+    <t>Csl-Boca-PV-1</t>
+  </si>
+  <si>
+    <t>JN420361</t>
+  </si>
+  <si>
+    <t>Zalophus californianus</t>
+  </si>
+  <si>
+    <t>Capra hircus</t>
+  </si>
+  <si>
+    <t>Porcine bocavirus 4-1</t>
+  </si>
+  <si>
+    <t>Prc-Boca-PV-4-1</t>
+  </si>
+  <si>
+    <t>JF429835</t>
+  </si>
+  <si>
+    <t>Rhinolophus pusillus bocaparvovirus 1</t>
+  </si>
+  <si>
+    <t>MF682922</t>
+  </si>
+  <si>
+    <t>Rhinolophus pusillus</t>
+  </si>
+  <si>
+    <t>Rp-Boca-PV-1</t>
+  </si>
+  <si>
+    <t>Rhinolophus pusillus bocaparvovirus 2</t>
+  </si>
+  <si>
+    <t>Rp-Boca-PV-2</t>
+  </si>
+  <si>
+    <t>MF682923</t>
+  </si>
+  <si>
+    <t>Deer tetraparvovirus</t>
+  </si>
+  <si>
+    <t>Deer-TetraPV</t>
+  </si>
+  <si>
+    <t>NC_031670</t>
+  </si>
+  <si>
+    <t>Ovine hokovirus 1</t>
+  </si>
+  <si>
+    <t>JF504699</t>
+  </si>
+  <si>
+    <t>Ovine-TetraPV</t>
+  </si>
+  <si>
+    <t>Ovis aries</t>
+  </si>
+  <si>
+    <t>EU200669</t>
+  </si>
+  <si>
+    <t>Bovine hokovirus</t>
+  </si>
+  <si>
+    <t>Bovine-TetraPV</t>
+  </si>
+  <si>
+    <t>Porcine hokovirus</t>
+  </si>
+  <si>
+    <t>Porcine-TetraPV</t>
+  </si>
+  <si>
+    <t>EU200677</t>
+  </si>
+  <si>
+    <t>Chimpanzee parv4</t>
+  </si>
+  <si>
+    <t>Pan troglodytes</t>
+  </si>
+  <si>
+    <t>HQ113143</t>
+  </si>
+  <si>
+    <t>Chimp-Parv-4</t>
+  </si>
+  <si>
+    <t>AY622943</t>
+  </si>
+  <si>
+    <t>Human parv4</t>
+  </si>
+  <si>
+    <t>Human-Parv-4</t>
+  </si>
+  <si>
+    <t>Rodent tetraparvovirus</t>
+  </si>
+  <si>
+    <t>MG745669</t>
+  </si>
+  <si>
+    <t>Rodent-TetraPV</t>
+  </si>
+  <si>
+    <t>Opossum tetraparvovirus</t>
+  </si>
+  <si>
+    <t>Opossum-TetraPV</t>
+  </si>
+  <si>
+    <t>MG745671</t>
+  </si>
+  <si>
+    <t>Parvovirus YX-2010</t>
+  </si>
+  <si>
+    <t>GU938300</t>
+  </si>
+  <si>
+    <t>MG972981</t>
+  </si>
+  <si>
+    <t>Ungulate copiparvovirus 1</t>
+  </si>
+  <si>
+    <t>Ungulate-Copi-PV-1</t>
+  </si>
+  <si>
+    <t>Chipmunk parvovirus</t>
+  </si>
+  <si>
+    <t>GQ200736</t>
+  </si>
+  <si>
+    <t>Rhesus macaque parvovirus</t>
+  </si>
+  <si>
+    <t>AF221122</t>
+  </si>
+  <si>
+    <t>AF221123</t>
+  </si>
+  <si>
+    <t>Pig-tailed macaque parvovirus</t>
+  </si>
+  <si>
+    <t>Simian parvovirus</t>
+  </si>
+  <si>
+    <t>U26342</t>
+  </si>
+  <si>
+    <t>Macaca fascicularis</t>
+  </si>
+  <si>
+    <t>Bovine parvovirus 3</t>
+  </si>
+  <si>
+    <t>AF406967</t>
+  </si>
+  <si>
+    <t>Cebus_imitator.1</t>
+  </si>
+  <si>
+    <t>Mesitornis_unicolor.1</t>
+  </si>
+  <si>
+    <t>Myotis_davidii.1</t>
+  </si>
+  <si>
+    <t>Protobothrops_mucrosquamatus.1</t>
+  </si>
+  <si>
+    <t>Serinus_canaria.1</t>
+  </si>
+  <si>
+    <t>Giraffa_tippelskirchi.1</t>
+  </si>
+  <si>
+    <t>Cebus imitator</t>
+  </si>
+  <si>
+    <t>Mesitornis unicolor</t>
+  </si>
+  <si>
+    <t>Myotis davidii</t>
+  </si>
+  <si>
+    <t>Protobothrops mucrosquamatus</t>
+  </si>
+  <si>
+    <t>Serinus canaria</t>
+  </si>
+  <si>
+    <t>Giraffa tippelskirchi</t>
+  </si>
+  <si>
+    <t>MH670587</t>
+  </si>
+  <si>
+    <t>Mouse kidney parvovirus</t>
+  </si>
+  <si>
+    <t>Mk-PV</t>
+  </si>
+  <si>
+    <t>Macaca nemestrina</t>
+  </si>
+  <si>
+    <t>Macaca mulatta</t>
+  </si>
+  <si>
+    <t>Simian-PV</t>
+  </si>
+  <si>
+    <t>Simian-PV-pgm</t>
+  </si>
+  <si>
+    <t>Simian-PV-rm</t>
+  </si>
+  <si>
+    <t>Chipmunk-PV</t>
+  </si>
+  <si>
+    <t>Bovine-PV-3</t>
+  </si>
+  <si>
+    <t>PPV-NADL-2</t>
+  </si>
+  <si>
+    <t>EU659112</t>
+  </si>
+  <si>
+    <t>Feline panleukopenia virus</t>
+  </si>
+  <si>
+    <t>Felis catus</t>
+  </si>
+  <si>
+    <t>FPV</t>
+  </si>
+  <si>
+    <t>Eidolon helvum parvovirus 2</t>
+  </si>
+  <si>
+    <t>Unclassified-5</t>
+  </si>
+  <si>
+    <t>JX885610</t>
+  </si>
+  <si>
+    <t>Eh-PV-2</t>
   </si>
 </sst>
 </file>
@@ -572,7 +884,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -609,6 +921,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -619,7 +937,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="381">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -773,8 +1091,236 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -787,8 +1333,14 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="381">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -865,6 +1417,120 @@
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -941,6 +1607,120 @@
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1270,10 +2050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F41" sqref="A1:F41"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C76" sqref="C75:C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1307,14 +2087,14 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>93</v>
+      <c r="A2" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>237</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>96</v>
@@ -1322,770 +2102,1397 @@
       <c r="E2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>123</v>
+      <c r="A4" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>122</v>
+      <c r="A5" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="A6" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>121</v>
+      <c r="A7" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1"/>
+      <c r="A8" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>119</v>
+      <c r="A9" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>104</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B18" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C18" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="D18" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F18" s="15" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B21" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C21" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="D21" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>147</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>114</v>
-      </c>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="A22" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="4" t="s">
-        <v>50</v>
+      <c r="A24" t="s">
+        <v>147</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>74</v>
+        <v>148</v>
+      </c>
+      <c r="C24" t="s">
+        <v>146</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
-        <v>54</v>
+        <v>135</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>55</v>
+        <v>140</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="4" t="s">
-        <v>88</v>
+      <c r="A29" t="s">
+        <v>182</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>90</v>
+        <v>181</v>
+      </c>
+      <c r="C29" t="s">
+        <v>180</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>117</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
-        <v>57</v>
+        <v>187</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>58</v>
+        <v>186</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>78</v>
+        <v>185</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="4" t="s">
-        <v>62</v>
+      <c r="A32" t="s">
+        <v>179</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>76</v>
+        <v>178</v>
+      </c>
+      <c r="C32" t="s">
+        <v>176</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>113</v>
+        <v>33</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" t="s">
-        <v>152</v>
+      <c r="A33" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>36</v>
+        <v>191</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>113</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
-        <v>142</v>
+        <v>194</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F34" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
-        <v>22</v>
+        <v>128</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>81</v>
+        <v>127</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>115</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" t="s">
-        <v>150</v>
+      <c r="A36" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C36" t="s">
-        <v>149</v>
+        <v>42</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>24</v>
+      <c r="E36" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="4" t="s">
-        <v>108</v>
+      <c r="A37" t="s">
+        <v>223</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>105</v>
+        <v>225</v>
+      </c>
+      <c r="C37" t="s">
+        <v>224</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>110</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>139</v>
+        <v>46</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>136</v>
+        <v>64</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F38" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" t="s">
-        <v>154</v>
+      <c r="A39" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C39" t="s">
-        <v>153</v>
+        <v>49</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E40" s="5" t="s">
+      <c r="D51" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F40" s="5" t="s">
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F53" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>162</v>
-      </c>
-      <c r="B41" t="s">
-        <v>161</v>
-      </c>
-      <c r="C41" t="s">
-        <v>160</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41" s="5" t="s">
+    <row r="54" spans="1:6">
+      <c r="A54" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F41" s="10" t="s">
-        <v>163</v>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F59" s="5"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>212</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>220</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C65" t="s">
+        <v>218</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
+        <v>222</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="C67" t="s">
+        <v>221</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>216</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" t="s">
+        <v>215</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>266</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C73" t="s">
+        <v>264</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F38">
-    <sortCondition ref="D2:D38"/>
-    <sortCondition ref="E2:E38"/>
-    <sortCondition ref="B2:B38"/>
+  <sortState ref="A2:F71">
+    <sortCondition ref="D2:D71"/>
+    <sortCondition ref="E2:E71"/>
+    <sortCondition ref="B2:B71"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Updated taxonomic data for sesavirus
</commit_message>
<xml_diff>
--- a/tabular/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/parvo-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15860" yWindow="5300" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3920" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal refset" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="269">
   <si>
     <t>accession-ID</t>
   </si>
@@ -824,6 +824,9 @@
   </si>
   <si>
     <t>Eh-PV-2</t>
+  </si>
+  <si>
+    <t>Marinoparvovirus</t>
   </si>
 </sst>
 </file>
@@ -884,7 +887,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -917,13 +920,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDEF3A8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFADFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE9D7C8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1320,7 +1341,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1332,13 +1353,22 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="381">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2052,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C76" sqref="C75:C76"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2087,13 +2117,13 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>237</v>
       </c>
       <c r="D2" s="8" t="s">
@@ -2127,13 +2157,13 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>242</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -2147,13 +2177,13 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>238</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -2167,13 +2197,13 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>250</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -2187,13 +2217,13 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>239</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -2207,13 +2237,13 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>240</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -2227,13 +2257,13 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>241</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -2403,100 +2433,100 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="15" t="s">
+      <c r="D18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="13" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="15" t="s">
+      <c r="D19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="15" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="15" t="s">
+      <c r="D20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="13" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="15" t="s">
+      <c r="D21" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="15"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="15" t="s">
+      <c r="D22" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="17"/>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
@@ -2519,220 +2549,220 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" t="s">
+      <c r="A24" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="5" t="s">
+      <c r="D24" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="D25" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="18" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="5" t="s">
+      <c r="D26" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="18" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="D27" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="18" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="D28" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="18" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" t="s">
+      <c r="A29" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="D29" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="18" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="5" t="s">
+      <c r="D30" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="18" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="D31" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="18" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" t="s">
+      <c r="A32" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="D32" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="19" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="5" t="s">
+      <c r="D33" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="18" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="5" t="s">
+      <c r="D34" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="18" t="s">
         <v>190</v>
       </c>
     </row>
@@ -2793,98 +2823,98 @@
       <c r="F37" s="10"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E38" s="5" t="s">
+      <c r="D38" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F38" s="21" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E39" s="5" t="s">
+      <c r="D39" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E39" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="21" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E40" s="5" t="s">
+      <c r="D40" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="5"/>
+      <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41" s="5" t="s">
+      <c r="D41" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E41" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="5"/>
+      <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="5" t="s">
+      <c r="D42" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F42" s="5"/>
+      <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
@@ -3005,198 +3035,198 @@
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E49" s="5" t="s">
+      <c r="D49" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="23" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E50" s="5" t="s">
+      <c r="D50" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F50" s="5" t="s">
+      <c r="F50" s="23" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" s="5" t="s">
+      <c r="D51" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F51" s="5"/>
+      <c r="F51" s="23"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="5" t="s">
+      <c r="D52" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F52" s="5" t="s">
+      <c r="F52" s="23" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E53" s="5" t="s">
+      <c r="D53" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F53" s="5" t="s">
+      <c r="F53" s="23" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" s="5" t="s">
+      <c r="D54" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F54" s="5"/>
+      <c r="F54" s="23"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E55" s="5" t="s">
+      <c r="D55" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F55" s="5" t="s">
+      <c r="F55" s="23" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" s="5" t="s">
+      <c r="D56" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F56" s="5" t="s">
+      <c r="F56" s="23" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="22" t="s">
         <v>261</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E57" s="5" t="s">
+      <c r="D57" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F57" s="5" t="s">
+      <c r="F57" s="23" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E58" s="5" t="s">
+      <c r="D58" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="F58" s="23" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3214,219 +3244,221 @@
         <v>27</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>141</v>
+        <v>268</v>
       </c>
       <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E60" s="11" t="s">
+      <c r="D60" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F60" s="5" t="s">
+      <c r="F60" s="25" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="4" t="s">
+      <c r="A61" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E61" s="11" t="s">
+      <c r="D61" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F61" s="5" t="s">
+      <c r="F61" s="25" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E62" s="11" t="s">
+      <c r="D62" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F62" s="5"/>
+      <c r="F62" s="25"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="4" t="s">
+      <c r="A63" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E63" s="5" t="s">
+      <c r="D63" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F63" s="5" t="s">
+      <c r="F63" s="25" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" t="s">
+      <c r="A64" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E64" s="11" t="s">
+      <c r="D64" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F64" s="5" t="s">
+      <c r="F64" s="25" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" t="s">
+      <c r="A65" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E65" s="11" t="s">
+      <c r="D65" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="25" t="s">
         <v>24</v>
       </c>
+      <c r="F65" s="26"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="4" t="s">
+      <c r="A66" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E66" s="11" t="s">
+      <c r="D66" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F66" s="5" t="s">
+      <c r="F66" s="25" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" t="s">
+      <c r="A67" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B67" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" s="11" t="s">
+      <c r="D67" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E67" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F67" s="5" t="s">
+      <c r="F67" s="25" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="D68" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E68" s="11" t="s">
+      <c r="D68" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F68" s="5" t="s">
+      <c r="F68" s="25" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" t="s">
+      <c r="A69" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E69" s="11" t="s">
+      <c r="D69" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69" s="25" t="s">
         <v>24</v>
       </c>
+      <c r="F69" s="26"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="4" t="s">
+      <c r="A70" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E70" s="11" t="s">
+      <c r="D70" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F70" s="5"/>
+      <c r="F70" s="25"/>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="4" t="s">

</xml_diff>

<commit_message>
Expanded dependoparvovirus reference set to include all AAVs + BdrPV
</commit_message>
<xml_diff>
--- a/tabular/parvo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/parvo-ncbi-refseqs-side-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="3920" yWindow="0" windowWidth="30680" windowHeight="25440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Minimal refset" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="325">
   <si>
     <t>accession-ID</t>
   </si>
@@ -827,6 +827,174 @@
   </si>
   <si>
     <t>Marinoparvovirus</t>
+  </si>
+  <si>
+    <t>AF028704</t>
+  </si>
+  <si>
+    <t>AF028705</t>
+  </si>
+  <si>
+    <t>AF085716</t>
+  </si>
+  <si>
+    <t>AX753250</t>
+  </si>
+  <si>
+    <t>AY243002</t>
+  </si>
+  <si>
+    <t>AY243021</t>
+  </si>
+  <si>
+    <t>AY243022</t>
+  </si>
+  <si>
+    <t>AY631966</t>
+  </si>
+  <si>
+    <t>DI393763</t>
+  </si>
+  <si>
+    <t>DQ813647</t>
+  </si>
+  <si>
+    <t>KT984498</t>
+  </si>
+  <si>
+    <t>LY408697</t>
+  </si>
+  <si>
+    <t>NC_001729</t>
+  </si>
+  <si>
+    <t>NC_001829</t>
+  </si>
+  <si>
+    <t>NC_002077</t>
+  </si>
+  <si>
+    <t>NC_006152</t>
+  </si>
+  <si>
+    <t>NC_006260</t>
+  </si>
+  <si>
+    <t>NC_006261</t>
+  </si>
+  <si>
+    <t>NC_027429</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 6</t>
+  </si>
+  <si>
+    <t>AAV6</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 3B</t>
+  </si>
+  <si>
+    <t>AAV3B</t>
+  </si>
+  <si>
+    <t>AAV5</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 5</t>
+  </si>
+  <si>
+    <t>AAV9</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 9</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 11</t>
+  </si>
+  <si>
+    <t>AAV11</t>
+  </si>
+  <si>
+    <t>NHP-AAV-type2</t>
+  </si>
+  <si>
+    <t>NHP-AAV-type1</t>
+  </si>
+  <si>
+    <t>NHP Adeno-associated virus 11</t>
+  </si>
+  <si>
+    <t>NHP Adeno-associated virus type 2</t>
+  </si>
+  <si>
+    <t>NHP Adeno-associated virus type 1</t>
+  </si>
+  <si>
+    <t>NHP-AAV11</t>
+  </si>
+  <si>
+    <t>AAV4</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 4</t>
+  </si>
+  <si>
+    <t>AAV12</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 12</t>
+  </si>
+  <si>
+    <t>NHP Adeno-associated virus 6</t>
+  </si>
+  <si>
+    <t>NHP-AAV6</t>
+  </si>
+  <si>
+    <t>AAV10</t>
+  </si>
+  <si>
+    <t>AAV3</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 3</t>
+  </si>
+  <si>
+    <t>AAV1</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 1</t>
+  </si>
+  <si>
+    <t>AAV7</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 7</t>
+  </si>
+  <si>
+    <t>AAV8</t>
+  </si>
+  <si>
+    <t>Adeno-associated virus 8</t>
+  </si>
+  <si>
+    <t>Bearded dragon parvovirus strain 2014</t>
+  </si>
+  <si>
+    <t>BdrPV</t>
+  </si>
+  <si>
+    <t>Cairina moschata</t>
+  </si>
+  <si>
+    <t>Anser anser</t>
+  </si>
+  <si>
+    <t>Python regius</t>
+  </si>
+  <si>
+    <t>Tamias sibiricus</t>
   </si>
 </sst>
 </file>
@@ -887,7 +1055,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -948,6 +1116,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6699FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -958,7 +1144,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="381">
+  <cellStyleXfs count="613">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1340,8 +1526,240 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1369,8 +1787,16 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="381">
+  <cellStyles count="613">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1561,6 +1987,122 @@
     <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="474" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="476" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="478" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="480" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="482" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="484" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="486" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="488" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="490" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="492" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="494" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="496" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="498" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="500" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="502" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="504" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="506" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="508" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="510" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="512" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="514" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="516" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="518" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="520" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="522" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="524" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="536" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1751,6 +2293,122 @@
     <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="473" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="475" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="477" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="479" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="481" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="483" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="485" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="487" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="489" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="491" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="493" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="495" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="497" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="499" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="501" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="503" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="505" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="507" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="509" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="511" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="513" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="515" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="517" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="519" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="521" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="523" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="535" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2080,10 +2738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="L70" sqref="L70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2529,22 +3187,22 @@
       <c r="F22" s="15"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="D23" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="34" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2767,70 +3425,70 @@
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="5" t="s">
+      <c r="D35" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="F35" s="5"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="5" t="s">
+      <c r="D36" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F36" s="5" t="s">
+      <c r="F36" s="28" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" t="s">
+      <c r="A37" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="5" t="s">
+      <c r="D37" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F37" s="10"/>
+      <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="20" t="s">
-        <v>45</v>
+        <v>283</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>46</v>
+        <v>313</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>64</v>
+        <v>314</v>
       </c>
       <c r="D38" s="21" t="s">
         <v>27</v>
@@ -2844,13 +3502,13 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="20" t="s">
-        <v>48</v>
+        <v>280</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>49</v>
+        <v>310</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>71</v>
+        <v>296</v>
       </c>
       <c r="D39" s="21" t="s">
         <v>27</v>
@@ -2859,18 +3517,18 @@
         <v>44</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>184</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="20" t="s">
-        <v>50</v>
+        <v>276</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>51</v>
+        <v>297</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>74</v>
+        <v>296</v>
       </c>
       <c r="D40" s="21" t="s">
         <v>27</v>
@@ -2878,17 +3536,19 @@
       <c r="E40" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="21"/>
+      <c r="F40" s="21" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="20" t="s">
-        <v>52</v>
+        <v>278</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>53</v>
+        <v>306</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>80</v>
+        <v>307</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>27</v>
@@ -2896,17 +3556,19 @@
       <c r="E41" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="21"/>
+      <c r="F41" s="21" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D42" s="21" t="s">
         <v>27</v>
@@ -2914,617 +3576,1001 @@
       <c r="E42" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F42" s="21"/>
+      <c r="F42" s="21" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="D48" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>315</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C62" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="5" t="s">
+      <c r="D62" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F43" s="5" t="s">
+      <c r="F62" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44" s="4" t="s">
+    <row r="63" spans="1:6">
+      <c r="A63" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B63" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="5" t="s">
+      <c r="D63" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F44" s="5" t="s">
+      <c r="F63" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="4" t="s">
+    <row r="64" spans="1:6">
+      <c r="A64" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B64" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" s="5" t="s">
+      <c r="D64" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F45" s="5"/>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="4" t="s">
+      <c r="F64" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B65" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C65" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E46" s="5" t="s">
+      <c r="D65" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F65" s="5" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47" s="4" t="s">
+    <row r="66" spans="1:6">
+      <c r="A66" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E47" s="5" t="s">
+      <c r="D66" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F66" s="5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
-      <c r="A48" s="4" t="s">
+    <row r="67" spans="1:6">
+      <c r="A67" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" s="5" t="s">
+      <c r="D67" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F67" s="5" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="22" t="s">
+    <row r="68" spans="1:6">
+      <c r="A68" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="F68" s="8"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B69" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="C49" s="22" t="s">
+      <c r="C69" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="D49" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E49" s="23" t="s">
+      <c r="D69" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E69" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F49" s="23" t="s">
+      <c r="F69" s="23" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="22" t="s">
+    <row r="70" spans="1:6">
+      <c r="A70" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B70" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C70" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="D50" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E50" s="23" t="s">
+      <c r="D70" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E70" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F50" s="23" t="s">
+      <c r="F70" s="23" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="22" t="s">
+    <row r="71" spans="1:6">
+      <c r="A71" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="C71" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="D71" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F71" s="23" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B72" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="C51" s="22" t="s">
+      <c r="C72" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="D51" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="E51" s="23" t="s">
+      <c r="D72" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E72" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F51" s="23"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="22" t="s">
+      <c r="F72" s="23"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="22" t="s">
+      <c r="B73" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C52" s="22" t="s">
+      <c r="C73" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D52" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E52" s="23" t="s">
+      <c r="D73" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E73" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F52" s="23" t="s">
+      <c r="F73" s="23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="22" t="s">
+    <row r="74" spans="1:6">
+      <c r="A74" s="22" t="s">
         <v>154</v>
       </c>
-      <c r="B53" s="22" t="s">
+      <c r="B74" s="22" t="s">
         <v>155</v>
       </c>
-      <c r="C53" s="22" t="s">
+      <c r="C74" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="D53" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E53" s="23" t="s">
+      <c r="D74" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E74" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F53" s="23" t="s">
+      <c r="F74" s="23" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="22" t="s">
+    <row r="75" spans="1:6">
+      <c r="A75" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B54" s="22" t="s">
+      <c r="B75" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C75" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="D54" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E54" s="23" t="s">
+      <c r="D75" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E75" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F54" s="23"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="22" t="s">
+      <c r="F75" s="23"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B76" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="22" t="s">
+      <c r="C76" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E55" s="23" t="s">
+      <c r="D76" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E76" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F55" s="23" t="s">
+      <c r="F76" s="23" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="22" t="s">
+    <row r="77" spans="1:6">
+      <c r="A77" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B77" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="22" t="s">
+      <c r="C77" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="D56" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E56" s="23" t="s">
+      <c r="D77" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E77" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F56" s="23" t="s">
+      <c r="F77" s="23" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="22" t="s">
-        <v>260</v>
-      </c>
-      <c r="B57" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="D57" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E57" s="23" t="s">
+    <row r="78" spans="1:6">
+      <c r="A78" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E78" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F57" s="23" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="B58" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E58" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F58" s="23" t="s">
+      <c r="F78" s="23" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="F59" s="5"/>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="24" t="s">
+    <row r="79" spans="1:6">
+      <c r="A79" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="B60" s="24" t="s">
+      <c r="B79" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="C60" s="24" t="s">
+      <c r="C79" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="D60" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E60" s="25" t="s">
+      <c r="D79" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E79" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F60" s="25" t="s">
+      <c r="F79" s="25" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="24" t="s">
+    <row r="80" spans="1:6">
+      <c r="A80" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="B61" s="24" t="s">
+      <c r="B80" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="C61" s="24" t="s">
+      <c r="C80" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="D61" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E61" s="25" t="s">
+      <c r="D80" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E80" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F61" s="25" t="s">
+      <c r="F80" s="25" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="24" t="s">
+    <row r="81" spans="1:6">
+      <c r="A81" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="B81" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="C62" s="24" t="s">
+      <c r="C81" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="D62" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E62" s="25" t="s">
+      <c r="D81" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E81" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F62" s="25"/>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="24" t="s">
+      <c r="F81" s="25"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B63" s="24" t="s">
+      <c r="B82" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="24" t="s">
+      <c r="C82" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="D63" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E63" s="25" t="s">
+      <c r="D82" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E82" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F63" s="25" t="s">
+      <c r="F82" s="25" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="26" t="s">
+    <row r="83" spans="1:6">
+      <c r="A83" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B83" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C83" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="D64" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E64" s="25" t="s">
+      <c r="D83" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E83" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F64" s="25" t="s">
+      <c r="F83" s="25" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="26" t="s">
+    <row r="84" spans="1:6">
+      <c r="A84" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="B65" s="24" t="s">
+      <c r="B84" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="C65" s="26" t="s">
+      <c r="C84" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="D65" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E65" s="25" t="s">
+      <c r="D84" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E84" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F65" s="26"/>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="24" t="s">
+      <c r="F84" s="26"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="B66" s="24" t="s">
+      <c r="B85" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="C66" s="24" t="s">
+      <c r="C85" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="D66" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E66" s="25" t="s">
+      <c r="D85" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E85" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F66" s="25" t="s">
+      <c r="F85" s="25" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="26" t="s">
+    <row r="86" spans="1:6">
+      <c r="A86" s="26" t="s">
         <v>222</v>
       </c>
-      <c r="B67" s="24" t="s">
+      <c r="B86" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="C67" s="26" t="s">
+      <c r="C86" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="D67" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" s="25" t="s">
+      <c r="D86" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E86" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F67" s="25" t="s">
+      <c r="F86" s="25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="24" t="s">
+    <row r="87" spans="1:6">
+      <c r="A87" s="24" t="s">
         <v>207</v>
       </c>
-      <c r="B68" s="24" t="s">
+      <c r="B87" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="C68" s="24" t="s">
+      <c r="C87" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="D68" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E68" s="25" t="s">
+      <c r="D87" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E87" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F68" s="25" t="s">
+      <c r="F87" s="25" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="26" t="s">
+    <row r="88" spans="1:6">
+      <c r="A88" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="B69" s="24" t="s">
+      <c r="B88" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="C69" s="26" t="s">
+      <c r="C88" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="D69" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E69" s="25" t="s">
+      <c r="D88" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E88" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F69" s="26"/>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="24" t="s">
+      <c r="F88" s="26"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="B70" s="24" t="s">
+      <c r="B89" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="C70" s="24" t="s">
+      <c r="C89" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="D70" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E70" s="25" t="s">
+      <c r="D89" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E89" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F70" s="25"/>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="4" t="s">
+      <c r="F89" s="25"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E71" s="5" t="s">
+      <c r="D90" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F71" s="5" t="s">
+      <c r="F90" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="4" t="s">
+    <row r="91" spans="1:6">
+      <c r="A91" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B91" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C91" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D72" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E72" s="5" t="s">
+      <c r="D91" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E91" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="F72" s="5" t="s">
+      <c r="F91" s="5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
-      <c r="A73" t="s">
+    <row r="92" spans="1:6">
+      <c r="A92" t="s">
         <v>266</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B92" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C92" t="s">
         <v>264</v>
       </c>
-      <c r="D73" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E73" s="5" t="s">
+      <c r="D92" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E92" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="F73" s="10" t="s">
+      <c r="F92" s="10" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F71">
-    <sortCondition ref="D2:D71"/>
-    <sortCondition ref="E2:E71"/>
-    <sortCondition ref="B2:B71"/>
+  <sortState ref="A2:F92">
+    <sortCondition ref="D2:D92"/>
+    <sortCondition ref="E2:E92"/>
+    <sortCondition ref="B2:B92"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>